<commit_message>
new version. rough implementation of transactional file. so far only working for daily T&A report with reservations...
</commit_message>
<xml_diff>
--- a/CARD USER I.D LIST 2.xlsx
+++ b/CARD USER I.D LIST 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\josom\exegui_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC37A4BF-6BD6-4273-92E9-EFD22236715E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0B5AD8-59EC-4FD9-A0CE-528D644B9714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5655" yWindow="945" windowWidth="21435" windowHeight="14745" tabRatio="531" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1455" windowWidth="21435" windowHeight="14745" tabRatio="531" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6802" uniqueCount="1441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6803" uniqueCount="1442">
   <si>
     <t>Card N°.</t>
   </si>
@@ -4347,6 +4347,9 @@
   </si>
   <si>
     <t>HOTEL SECURITY (TRAFFIC)</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -30376,10 +30379,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD48ACC-20CB-4805-A8E3-95FADC56D8B5}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30412,7 +30415,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>1441</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -30429,7 +30432,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1390</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -30446,7 +30449,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1386</v>
+        <v>1390</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -30463,7 +30466,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -30480,7 +30483,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -30497,7 +30500,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1424</v>
+        <v>1391</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -30514,69 +30517,69 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1423</v>
+        <v>1425</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>19</v>
-      </c>
-      <c r="E9">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1340</v>
+        <v>1423</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E10">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1382</v>
+        <v>1340</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1426</v>
+        <v>1382</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -30593,41 +30596,41 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E13">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1344</v>
+        <v>1427</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C14">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>1344</v>
       </c>
       <c r="B15">
         <v>7</v>
@@ -30644,75 +30647,75 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1381</v>
+        <v>27</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D16">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1385</v>
+        <v>1381</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1440</v>
+        <v>1385</v>
       </c>
       <c r="B18">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E18">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C19">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1421</v>
+        <v>1439</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -30729,132 +30732,149 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1383</v>
+        <v>1421</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>18</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1428</v>
-      </c>
-      <c r="B22">
-        <v>7</v>
-      </c>
-      <c r="C22">
-        <v>19</v>
-      </c>
-      <c r="D22">
-        <v>19</v>
-      </c>
-      <c r="E22">
-        <v>7</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E23">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1388</v>
+        <v>1429</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C24">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1420</v>
+        <v>1388</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>19</v>
+      </c>
+      <c r="D25">
+        <v>19</v>
+      </c>
+      <c r="E25">
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1387</v>
-      </c>
-      <c r="B26">
-        <v>12</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>12</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1430</v>
+        <v>1387</v>
       </c>
       <c r="B27">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C27">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1353</v>
+        <v>1430</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C28">
-        <v>19</v>
-      </c>
-      <c r="D28">
-        <v>19</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1432</v>
-      </c>
-      <c r="F29" t="s">
-        <v>1431</v>
+        <v>1353</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>19</v>
+      </c>
+      <c r="D29">
+        <v>19</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>1432</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>1433</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>7</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>19</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>19</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove usere from reportr if no in or out for the cutoff
</commit_message>
<xml_diff>
--- a/CARD USER I.D LIST 2.xlsx
+++ b/CARD USER I.D LIST 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\josom\exegui_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0B5AD8-59EC-4FD9-A0CE-528D644B9714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EAA49B-C87C-4CB7-91BB-075BEB701A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1455" windowWidth="21435" windowHeight="14745" tabRatio="531" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1215" yWindow="1065" windowWidth="26670" windowHeight="14745" tabRatio="531" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -30381,8 +30381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD48ACC-20CB-4805-A8E3-95FADC56D8B5}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30751,6 +30751,18 @@
       <c r="A22" t="s">
         <v>1383</v>
       </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <v>19</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -30806,6 +30818,18 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1420</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>19</v>
+      </c>
+      <c r="D26">
+        <v>19</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
enroll jkk and 8arms
</commit_message>
<xml_diff>
--- a/CARD USER I.D LIST 2.xlsx
+++ b/CARD USER I.D LIST 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\josom\exegui_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{724148BC-5F2E-4B76-9509-860D2E0AB0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E6462C-6DD6-4430-9563-9DBCBD091579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="1050" windowWidth="21600" windowHeight="11505" tabRatio="531" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" tabRatio="531" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KENICHI" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <sheet name="SNIFFER K9" sheetId="4" r:id="rId3"/>
     <sheet name="NESA" sheetId="5" r:id="rId4"/>
     <sheet name="ADVANCE" sheetId="6" r:id="rId5"/>
-    <sheet name="Schedules" sheetId="2" r:id="rId6"/>
+    <sheet name="8ARMS" sheetId="8" r:id="rId6"/>
+    <sheet name="JKK" sheetId="7" r:id="rId7"/>
+    <sheet name="Schedules" sheetId="2" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KENICHI!$A$1:$Q$350</definedName>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6061" uniqueCount="1071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6629" uniqueCount="1071">
   <si>
     <t>Card N°.</t>
   </si>
@@ -24221,7 +24223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E824BD-15A3-4393-B3BE-0B22ED1850DD}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -26948,11 +26950,2239 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0924B473-FEBA-4ADD-B90A-B699F41A864C}">
+  <dimension ref="A1:Q21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>730</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E3" s="2">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3">
+        <v>44937.733564814815</v>
+      </c>
+      <c r="G3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>747</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E4" s="2">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44939.771134259259</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E5" s="2">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44947.593518518515</v>
+      </c>
+      <c r="G5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E6" s="2">
+        <v>31</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44968.853749999995</v>
+      </c>
+      <c r="G6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E7" s="2">
+        <v>31</v>
+      </c>
+      <c r="F7" s="3">
+        <v>44968.855370370366</v>
+      </c>
+      <c r="G7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E8" s="2">
+        <v>31</v>
+      </c>
+      <c r="F8" s="3">
+        <v>44968.856134259258</v>
+      </c>
+      <c r="G8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E9" s="2">
+        <v>31</v>
+      </c>
+      <c r="F9" s="3">
+        <v>44968.856909722221</v>
+      </c>
+      <c r="G9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E10" s="2">
+        <v>31</v>
+      </c>
+      <c r="F10" s="3">
+        <v>44968.857430555552</v>
+      </c>
+      <c r="G10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E11" s="2">
+        <v>31</v>
+      </c>
+      <c r="F11" s="3">
+        <v>44968.857951388884</v>
+      </c>
+      <c r="G11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E12" s="2">
+        <v>31</v>
+      </c>
+      <c r="F12" s="3">
+        <v>44968.862164351849</v>
+      </c>
+      <c r="G12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E13" s="2">
+        <v>31</v>
+      </c>
+      <c r="F13" s="3">
+        <v>44968.862893518519</v>
+      </c>
+      <c r="G13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E14" s="2">
+        <v>31</v>
+      </c>
+      <c r="F14" s="3">
+        <v>44968.863715277774</v>
+      </c>
+      <c r="G14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E15" s="2">
+        <v>31</v>
+      </c>
+      <c r="F15" s="3">
+        <v>44968.864687499998</v>
+      </c>
+      <c r="G15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E16" s="2">
+        <v>31</v>
+      </c>
+      <c r="F16" s="3">
+        <v>44968.865231481483</v>
+      </c>
+      <c r="G16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E17" s="2">
+        <v>31</v>
+      </c>
+      <c r="F17" s="3">
+        <v>44968.866064814814</v>
+      </c>
+      <c r="G17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E18" s="2">
+        <v>31</v>
+      </c>
+      <c r="F18" s="3">
+        <v>44968.866643518515</v>
+      </c>
+      <c r="G18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E19" s="2">
+        <v>31</v>
+      </c>
+      <c r="F19" s="3">
+        <v>44968.867673611108</v>
+      </c>
+      <c r="G19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E20" s="2">
+        <v>31</v>
+      </c>
+      <c r="F20" s="3">
+        <v>44968.868229166663</v>
+      </c>
+      <c r="G20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E21" s="2">
+        <v>28</v>
+      </c>
+      <c r="F21" s="3">
+        <v>44986.701377314814</v>
+      </c>
+      <c r="G21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC776C6-BC4C-4274-8276-BFCE6ED1C0EA}">
+  <dimension ref="A1:Q21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>730</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E3" s="2">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3">
+        <v>44937.733564814815</v>
+      </c>
+      <c r="G3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>747</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E4" s="2">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44939.771134259259</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E5" s="2">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44947.593518518515</v>
+      </c>
+      <c r="G5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E6" s="2">
+        <v>31</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44968.853749999995</v>
+      </c>
+      <c r="G6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E7" s="2">
+        <v>31</v>
+      </c>
+      <c r="F7" s="3">
+        <v>44968.855370370366</v>
+      </c>
+      <c r="G7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E8" s="2">
+        <v>31</v>
+      </c>
+      <c r="F8" s="3">
+        <v>44968.856134259258</v>
+      </c>
+      <c r="G8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E9" s="2">
+        <v>31</v>
+      </c>
+      <c r="F9" s="3">
+        <v>44968.856909722221</v>
+      </c>
+      <c r="G9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E10" s="2">
+        <v>31</v>
+      </c>
+      <c r="F10" s="3">
+        <v>44968.857430555552</v>
+      </c>
+      <c r="G10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E11" s="2">
+        <v>31</v>
+      </c>
+      <c r="F11" s="3">
+        <v>44968.857951388884</v>
+      </c>
+      <c r="G11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E12" s="2">
+        <v>31</v>
+      </c>
+      <c r="F12" s="3">
+        <v>44968.862164351849</v>
+      </c>
+      <c r="G12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E13" s="2">
+        <v>31</v>
+      </c>
+      <c r="F13" s="3">
+        <v>44968.862893518519</v>
+      </c>
+      <c r="G13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E14" s="2">
+        <v>31</v>
+      </c>
+      <c r="F14" s="3">
+        <v>44968.863715277774</v>
+      </c>
+      <c r="G14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E15" s="2">
+        <v>31</v>
+      </c>
+      <c r="F15" s="3">
+        <v>44968.864687499998</v>
+      </c>
+      <c r="G15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E16" s="2">
+        <v>31</v>
+      </c>
+      <c r="F16" s="3">
+        <v>44968.865231481483</v>
+      </c>
+      <c r="G16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E17" s="2">
+        <v>31</v>
+      </c>
+      <c r="F17" s="3">
+        <v>44968.866064814814</v>
+      </c>
+      <c r="G17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E18" s="2">
+        <v>31</v>
+      </c>
+      <c r="F18" s="3">
+        <v>44968.866643518515</v>
+      </c>
+      <c r="G18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E19" s="2">
+        <v>31</v>
+      </c>
+      <c r="F19" s="3">
+        <v>44968.867673611108</v>
+      </c>
+      <c r="G19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E20" s="2">
+        <v>31</v>
+      </c>
+      <c r="F20" s="3">
+        <v>44968.868229166663</v>
+      </c>
+      <c r="G20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E21" s="2">
+        <v>28</v>
+      </c>
+      <c r="F21" s="3">
+        <v>44986.701377314814</v>
+      </c>
+      <c r="G21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD48ACC-20CB-4805-A8E3-95FADC56D8B5}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>